<commit_message>
Add displaying posts and their content
</commit_message>
<xml_diff>
--- a/JS-Frameworks-Self-Evaluation-Protocol.xlsx
+++ b/JS-Frameworks-Self-Evaluation-Protocol.xlsx
@@ -363,10 +363,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -642,7 +642,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -652,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,11 +717,11 @@
       <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
@@ -740,7 +740,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="6">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>18</v>
@@ -843,7 +843,9 @@
       <c r="B18" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="5"/>
+      <c r="C18" s="5">
+        <v>7</v>
+      </c>
       <c r="D18" s="5">
         <v>7</v>
       </c>
@@ -861,31 +863,31 @@
       </c>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="2:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="13" t="s">
         <v>41</v>
       </c>
       <c r="C20" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D20" s="5">
         <v>5</v>
       </c>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="2:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="13" t="s">
         <v>42</v>
       </c>
       <c r="C21" s="5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D21" s="5">
         <v>10</v>
       </c>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="2:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="13" t="s">
         <v>43</v>
       </c>
@@ -897,7 +899,7 @@
       </c>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="2:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="13" t="s">
         <v>44</v>
       </c>
@@ -909,7 +911,7 @@
       </c>
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="2:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="13" t="s">
         <v>45</v>
       </c>
@@ -1053,7 +1055,9 @@
       <c r="B36" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C36" s="7"/>
+      <c r="C36" s="7">
+        <v>0</v>
+      </c>
       <c r="D36" s="7">
         <v>10</v>
       </c>
@@ -1063,7 +1067,9 @@
       <c r="B37" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C37" s="7"/>
+      <c r="C37" s="7">
+        <v>0</v>
+      </c>
       <c r="D37" s="7">
         <v>5</v>
       </c>
@@ -1073,7 +1079,9 @@
       <c r="B38" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C38" s="7"/>
+      <c r="C38" s="7">
+        <v>0</v>
+      </c>
       <c r="D38" s="7">
         <v>10</v>
       </c>
@@ -1083,7 +1091,9 @@
       <c r="B39" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C39" s="7"/>
+      <c r="C39" s="7">
+        <v>0</v>
+      </c>
       <c r="D39" s="7">
         <v>5</v>
       </c>
@@ -1093,7 +1103,9 @@
       <c r="B40" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C40" s="7"/>
+      <c r="C40" s="7">
+        <v>0</v>
+      </c>
       <c r="D40" s="7">
         <v>5</v>
       </c>
@@ -1103,7 +1115,9 @@
       <c r="B41" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C41" s="7"/>
+      <c r="C41" s="7">
+        <v>0</v>
+      </c>
       <c r="D41" s="7">
         <v>5</v>
       </c>
@@ -1113,7 +1127,9 @@
       <c r="B42" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C42" s="7"/>
+      <c r="C42" s="7">
+        <v>0</v>
+      </c>
       <c r="D42" s="7">
         <v>20</v>
       </c>
@@ -1123,7 +1139,9 @@
       <c r="B43" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C43" s="7"/>
+      <c r="C43" s="7">
+        <v>0</v>
+      </c>
       <c r="D43" s="7">
         <v>10</v>
       </c>
@@ -1135,7 +1153,7 @@
       </c>
       <c r="C44" s="11">
         <f>SUM(C6:C43)</f>
-        <v>147</v>
+        <v>166</v>
       </c>
       <c r="D44" s="11">
         <v>370</v>

</xml_diff>